<commit_message>
Update data and data documentation
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD679B4-97FF-1F4C-B7F9-A73B3731F5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABEB8C1-857A-FF43-8BE9-DC8EDF0162D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="2600" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="9240" yWindow="3740" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t>file</t>
   </si>
@@ -49,9 +49,6 @@
     <t>notes</t>
   </si>
   <si>
-    <t>country.csv</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -107,13 +104,203 @@
   </si>
   <si>
     <t xml:space="preserve">The number of intermediate areas identified by the CIA World Factbook data. Note that while these data can be used to roughly estimate the number of administrative regions per country; this information is best supplemented by local expertise and information on the administrative organization of IHR-related activities. </t>
+  </si>
+  <si>
+    <t>country.tsv</t>
+  </si>
+  <si>
+    <t>unit_costs.tsv</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>default_value</t>
+  </si>
+  <si>
+    <t>The default value of the unit cost, in 2022 USD</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>The unit that the cost is measured in (e.g., per day, per year, per set, etc)</t>
+  </si>
+  <si>
+    <t>assumption</t>
+  </si>
+  <si>
+    <t>Written documentation of any key assumptions associated with the default cost</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>A URL, if any, associated with documented assumptions</t>
+  </si>
+  <si>
+    <t>The category of the cost (personnel, operating, or transport) based on the categorizations defined by Sloan et al in Sloan ML, Gleason BL, Squire JS, Koroma FF, Sogbeh SA, Park MJ. Cost Analysis of Health Facility Electronic Integrated Disease Surveillance and Response in One District in Sierra Leone. Health Security. 2020 Jan 1;18(S1):S-64-S-71.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Personnel costs </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">include salaries, benefits, and incentives (Sloan et al)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Operating costs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> include office supplies, utilities, building and equipment maintenance, rentals (Sloan et al) as well as operating costs for all capacities associated with the JEE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Transport costs </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>include costs associated with fuel and annual vehicle maintenance, vehicles, per diems, and lodging</t>
+    </r>
+  </si>
+  <si>
+    <t>The name of the default cost</t>
+  </si>
+  <si>
+    <t>A brief written description of the default cost</t>
+  </si>
+  <si>
+    <t>detailed_costing.tsv</t>
+  </si>
+  <si>
+    <t>cost_subcategory</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>unit_cost</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>The name of the costed unit, corresponding to a costed unit in unit_costs.tsv</t>
+  </si>
+  <si>
+    <t>The subcategory, if any, associated with the items</t>
+  </si>
+  <si>
+    <t>The item being costed as part of the unit cost</t>
+  </si>
+  <si>
+    <t>The number of items needed</t>
+  </si>
+  <si>
+    <t>The cost per unit</t>
+  </si>
+  <si>
+    <t>A reference, if any</t>
+  </si>
+  <si>
+    <t>An additional URL or a URL associated with the reference, if any</t>
+  </si>
+  <si>
+    <t>category_sloan</t>
+  </si>
+  <si>
+    <t>jee3.tsv</t>
+  </si>
+  <si>
+    <t>pillar</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>indicator</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>The pillar of global health security that the indicator/attribute correspond to: prevent, detect, respond, or "other"</t>
+  </si>
+  <si>
+    <t>The core capacity, as defined by the core capacities of JEE 3.0</t>
+  </si>
+  <si>
+    <t>The indicator, as defined by the indicators of JEE 3.0</t>
+  </si>
+  <si>
+    <t>The score associated with the specified attribute (1-5)</t>
+  </si>
+  <si>
+    <t>The attribute associated with the specified score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,6 +320,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -492,15 +687,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="57.83203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="175.33203125" style="4" customWidth="1"/>
@@ -523,97 +718,320 @@
     </row>
     <row r="2" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>54</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>54</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
+        <v>54</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>21</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add second edition SPAR data
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AF1C12-42AB-6A49-94A9-7E06DA3ADAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FFC717-949E-9B4D-BAF4-CE8CB65BF91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="1320" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>file</t>
   </si>
@@ -263,9 +263,6 @@
     <t>category_sloan</t>
   </si>
   <si>
-    <t>jee3.tsv</t>
-  </si>
-  <si>
     <t>pillar</t>
   </si>
   <si>
@@ -281,22 +278,43 @@
     <t>attribute</t>
   </si>
   <si>
-    <t>The pillar of global health security that the indicator/attribute correspond to: prevent, detect, respond, or "other"</t>
-  </si>
-  <si>
-    <t>The core capacity, as defined by the core capacities of JEE 3.0</t>
-  </si>
-  <si>
-    <t>The indicator, as defined by the indicators of JEE 3.0</t>
-  </si>
-  <si>
-    <t>The score associated with the specified attribute (1-5)</t>
-  </si>
-  <si>
-    <t>The attribute associated with the specified score</t>
-  </si>
-  <si>
-    <t>For more details, please see https://www.who.int/publications/i/item/9789240051980</t>
+    <t>metrics.tsv</t>
+  </si>
+  <si>
+    <t>This is the primary key of the table</t>
+  </si>
+  <si>
+    <t>framework</t>
+  </si>
+  <si>
+    <t>The name of the framework or system in which the metric is defined, including information on the edition (e.g., "JEE 3.0" or "SPAR 2.0")</t>
+  </si>
+  <si>
+    <t>metric_id</t>
+  </si>
+  <si>
+    <t>A unique ID associated with the specified metric</t>
+  </si>
+  <si>
+    <t>For more details, please see https://www.who.int/publications/i/item/9789240051980; note that the second edition SPAR (SPAR 2.0) does not explicitly define these pillars, for SPAR metrics, pillars were inferred by the research team based on pillar-indicator pairs as defined in the JEE</t>
+  </si>
+  <si>
+    <t>The pillar of global health security that the indicator/attribute correspond to; one of: Prevent, Detect, Respond, or IHR Related Hazards and Points of Entry and Border Health</t>
+  </si>
+  <si>
+    <t>For more details, please see  JEE or SPAR reference documents</t>
+  </si>
+  <si>
+    <t>The capacity associated with the metric</t>
+  </si>
+  <si>
+    <t>The indicator associated with the metric</t>
+  </si>
+  <si>
+    <t>The attribute that is required to obtain the specified score</t>
+  </si>
+  <si>
+    <t>A numeric score that assesses country performance</t>
   </si>
 </sst>
 </file>
@@ -394,7 +412,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -682,7 +700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -690,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -721,41 +739,38 @@
     </row>
     <row r="2" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>65</v>
@@ -763,86 +778,86 @@
     </row>
     <row r="5" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>6</v>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -850,10 +865,13 @@
         <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -861,13 +879,13 @@
         <v>23</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -875,38 +893,38 @@
         <v>23</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -914,10 +932,13 @@
         <v>24</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -925,10 +946,10 @@
         <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -936,10 +957,10 @@
         <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -947,10 +968,10 @@
         <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -958,32 +979,32 @@
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -991,10 +1012,10 @@
         <v>39</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1002,10 +1023,10 @@
         <v>39</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1013,10 +1034,10 @@
         <v>39</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1024,10 +1045,10 @@
         <v>39</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1035,10 +1056,10 @@
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1046,9 +1067,31 @@
         <v>39</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add initial data on Strengthening the Global Architecture for Health Emergency Preparedness, Response and Resilience metrics, data still partially complete and require additional data entry
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FFC717-949E-9B4D-BAF4-CE8CB65BF91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D573929-D520-7F47-B965-DB02E73A3D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="1320" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="4900" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>file</t>
   </si>
@@ -287,9 +287,6 @@
     <t>framework</t>
   </si>
   <si>
-    <t>The name of the framework or system in which the metric is defined, including information on the edition (e.g., "JEE 3.0" or "SPAR 2.0")</t>
-  </si>
-  <si>
     <t>metric_id</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
     <t>For more details, please see https://www.who.int/publications/i/item/9789240051980; note that the second edition SPAR (SPAR 2.0) does not explicitly define these pillars, for SPAR metrics, pillars were inferred by the research team based on pillar-indicator pairs as defined in the JEE</t>
   </si>
   <si>
-    <t>The pillar of global health security that the indicator/attribute correspond to; one of: Prevent, Detect, Respond, or IHR Related Hazards and Points of Entry and Border Health</t>
-  </si>
-  <si>
     <t>For more details, please see  JEE or SPAR reference documents</t>
   </si>
   <si>
@@ -311,10 +305,19 @@
     <t>The indicator associated with the metric</t>
   </si>
   <si>
-    <t>The attribute that is required to obtain the specified score</t>
-  </si>
-  <si>
-    <t>A numeric score that assesses country performance</t>
+    <t>The pillar or key system of global health security that the indicator/attribute correspond to; one of: Prevent, Detect, Respond, or IHR Related Hazards and Points of Entry and Border Health (for JEE SPAR), or Collaborative surveillance, Access to countermeasures, Emergency coordination, Clinical care, or Community protection (Global Architecture for Health Emergency Preparedness, Response and Resilience)</t>
+  </si>
+  <si>
+    <t>The name of the framework or system in which the metric is defined, including information on the edition (e.g., "JEE 3.0", "SPAR 2.0", "Health Emergency Preparedness, Response and Resilience (HEPR)")</t>
+  </si>
+  <si>
+    <t>A numeric score that assesses country performance against the metric</t>
+  </si>
+  <si>
+    <t>The attribute that is required to obtain the specified score on the metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For more details, please see  JEE or SPAR reference documents; note that the metrics within the Health Emergency Preparedness, Response and Resilience (HEPR) are not specifically scored, so no score will be indicated, only a written description of the desired capacity </t>
   </si>
 </sst>
 </file>
@@ -710,15 +713,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="57.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="74.33203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="175.33203125" style="4" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
@@ -742,10 +745,10 @@
         <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>60</v>
@@ -759,7 +762,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -770,10 +773,10 @@
         <v>54</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -784,10 +787,10 @@
         <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -798,10 +801,10 @@
         <v>56</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -812,10 +815,10 @@
         <v>57</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -826,10 +829,10 @@
         <v>58</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add explicit field documenting the source of intermediate area data -- currently all from cia world factbook
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D573929-D520-7F47-B965-DB02E73A3D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDBC180-CA89-3743-91DD-49F18BC8FE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4900" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="2600" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
   <si>
     <t>file</t>
   </si>
@@ -318,6 +318,15 @@
   </si>
   <si>
     <t xml:space="preserve">For more details, please see  JEE or SPAR reference documents; note that the metrics within the Health Emergency Preparedness, Response and Resilience (HEPR) are not specifically scored, so no score will be indicated, only a written description of the desired capacity </t>
+  </si>
+  <si>
+    <t>intermediate_area_reference</t>
+  </si>
+  <si>
+    <t>Metadata documenting the source (and date) based on which the intermediate area data were determined</t>
+  </si>
+  <si>
+    <t>Currently all intermediate data come from the CIA World Factbook (2022)</t>
   </si>
 </sst>
 </file>
@@ -711,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -896,10 +905,13 @@
         <v>23</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -907,10 +919,10 @@
         <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>20</v>
@@ -921,180 +933,191 @@
         <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add metric_id to line_items data and update data dictionary
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDBC180-CA89-3743-91DD-49F18BC8FE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CCCCCD-6533-3740-A160-8C3C123618B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="10120" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="103">
   <si>
     <t>file</t>
   </si>
@@ -327,6 +327,237 @@
   </si>
   <si>
     <t>Currently all intermediate data come from the CIA World Factbook (2022)</t>
+  </si>
+  <si>
+    <t>line_items.tsv</t>
+  </si>
+  <si>
+    <t>requirement</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>administrative_level</t>
+  </si>
+  <si>
+    <t>cost_type</t>
+  </si>
+  <si>
+    <t>custom_multiplier_1</t>
+  </si>
+  <si>
+    <t>custom_multiplier_1_units</t>
+  </si>
+  <si>
+    <t>custom_multiplier_2</t>
+  </si>
+  <si>
+    <t>custom_multiplier_2_units</t>
+  </si>
+  <si>
+    <t>relevant_references</t>
+  </si>
+  <si>
+    <t>optional_cost</t>
+  </si>
+  <si>
+    <t>notes_assumptions</t>
+  </si>
+  <si>
+    <t>Boolean (TRUE/FALSE) that indicates whether or not the cost is considered an "optional" cost based on an interpretation of the language in the JEE or other relevant metric</t>
+  </si>
+  <si>
+    <t>Any notes or additional assumptions made associated with the line item</t>
+  </si>
+  <si>
+    <t>Any additional references associated with the designation of the line item</t>
+  </si>
+  <si>
+    <t>A unique ID associated with the specified metric, which can be used to join to the metrics.tsv table</t>
+  </si>
+  <si>
+    <t>The requirement specified based on the attribute</t>
+  </si>
+  <si>
+    <t>The activity required to address the requirement</t>
+  </si>
+  <si>
+    <t>The unit cost associated with the activity</t>
+  </si>
+  <si>
+    <t>The units associated with that unit cost</t>
+  </si>
+  <si>
+    <t>A brief written description of the activity</t>
+  </si>
+  <si>
+    <t>Defines country geopolitical organization. For the purposes of costing IHR implementation, these are the administrative units that support public health efforts such as biosurveillance or emergency response. Administrative organization is divided between intermediate and local levels, including an optional second intermediate level for countries where such an organization exists.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Country: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">central or national-level government
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Intermediate (e.g., province, district): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Largest geopolitical unit under the central government
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Local (e.g., county, city): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Smallest geopolitical unit with a role in national public health prevention, detection, and response efforts
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Health facility: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Primarily expected to be hospitals and government-run health centers for the purposes of costing IHR implementation. Includes facilities participating in IHR-related activities including biosurveillance programs, point-of-care diagnostics for priorities diseases, prevention of healthcare associated infections, and biosafety and biosecurity programs.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Population:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Population, used to calculate costs for activities that scale with total population size (e.g., cost per vaccine dose)</t>
+    </r>
+  </si>
+  <si>
+    <t>Indicates whther the cost is a one-time/start up cost or a recurring cost. All recurring costs are assumed to be annual unless another (temporal) custom multiplier is specified.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">One-time </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">costs are needed once, assumed to be during year 1 or at startup
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Recurring </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>costs are needed multiple times, assumed to be annually unless another (temporal) custom multiplier is specified</t>
+    </r>
+  </si>
+  <si>
+    <t>A custom multiplier that can be used to adjust the cost of the line item, for example, specifying how many times an activity is needed per year, or how many days a meeting is, or how many software licenses are needed.</t>
+  </si>
+  <si>
+    <t>The units associated with the custom multiplier</t>
   </si>
 </sst>
 </file>
@@ -720,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1121,6 +1352,210 @@
         <v>52</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
initial commit of unit cost data
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CCCCCD-6533-3740-A160-8C3C123618B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8505CE26-2404-9B4D-8E7E-93254718DFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="6180" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="107">
   <si>
     <t>file</t>
   </si>
@@ -558,6 +558,18 @@
   </si>
   <si>
     <t>The units associated with the custom multiplier</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>subcategory</t>
+  </si>
+  <si>
+    <t>The category of the cost based on the cost categories defined by GHSS. Please see methods documentation for more detailed definitions</t>
+  </si>
+  <si>
+    <t>The subcategory of the cost based on the cost categories defined by GHSS. Please see methods documentation for more detailed definitions</t>
   </si>
 </sst>
 </file>
@@ -951,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1203,10 +1215,10 @@
         <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1214,10 +1226,10 @@
         <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>26</v>
+        <v>104</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1225,10 +1237,10 @@
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1236,10 +1248,10 @@
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1247,10 +1259,10 @@
         <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1258,32 +1270,32 @@
         <v>24</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1291,10 +1303,10 @@
         <v>39</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1302,10 +1314,10 @@
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1313,10 +1325,10 @@
         <v>39</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1324,10 +1336,10 @@
         <v>39</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1335,10 +1347,10 @@
         <v>39</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1346,32 +1358,32 @@
         <v>39</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1379,10 +1391,10 @@
         <v>76</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1390,10 +1402,10 @@
         <v>76</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1401,10 +1413,10 @@
         <v>76</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1412,10 +1424,10 @@
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1423,10 +1435,10 @@
         <v>76</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1434,10 +1446,10 @@
         <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1445,24 +1457,21 @@
         <v>76</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1470,24 +1479,24 @@
         <v>76</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1495,10 +1504,13 @@
         <v>76</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1506,7 +1518,7 @@
         <v>76</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>101</v>
@@ -1517,7 +1529,7 @@
         <v>76</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>102</v>
@@ -1528,10 +1540,10 @@
         <v>76</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1539,10 +1551,10 @@
         <v>76</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1550,9 +1562,31 @@
         <v>76</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add a UUID for each line item
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8505CE26-2404-9B4D-8E7E-93254718DFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B44FC35-5752-2245-B9E6-8FAEA9A35AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6180" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="110">
   <si>
     <t>file</t>
   </si>
@@ -570,6 +570,15 @@
   </si>
   <si>
     <t>The subcategory of the cost based on the cost categories defined by GHSS. Please see methods documentation for more detailed definitions</t>
+  </si>
+  <si>
+    <t>line_item_id</t>
+  </si>
+  <si>
+    <t>A universally unique identifier (UUID) for each line item</t>
+  </si>
+  <si>
+    <t>UUIDs generated using the R id package (https://cran.r-project.org/web/packages/ids/index.html), uuid function</t>
   </si>
 </sst>
 </file>
@@ -963,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1391,10 +1400,13 @@
         <v>76</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>91</v>
+        <v>108</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1402,10 +1414,10 @@
         <v>76</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,10 +1425,10 @@
         <v>76</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1424,10 +1436,10 @@
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1435,10 +1447,10 @@
         <v>76</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1446,10 +1458,10 @@
         <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1457,10 +1469,10 @@
         <v>76</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1468,10 +1480,10 @@
         <v>76</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1479,38 +1491,35 @@
         <v>76</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="3" t="s">
+    <row r="44" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1518,10 +1527,13 @@
         <v>76</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1529,10 +1541,10 @@
         <v>76</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1540,10 +1552,10 @@
         <v>76</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1551,10 +1563,10 @@
         <v>76</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1562,10 +1574,10 @@
         <v>76</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1573,10 +1585,10 @@
         <v>76</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1584,9 +1596,20 @@
         <v>76</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add two new administrative multipliers for poe and hcw
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B44FC35-5752-2245-B9E6-8FAEA9A35AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26EFF25-85F0-E94A-A7DD-E70748FE9C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="2600" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="112">
   <si>
     <t>file</t>
   </si>
@@ -395,6 +395,9 @@
     <t>Defines country geopolitical organization. For the purposes of costing IHR implementation, these are the administrative units that support public health efforts such as biosurveillance or emergency response. Administrative organization is divided between intermediate and local levels, including an optional second intermediate level for countries where such an organization exists.</t>
   </si>
   <si>
+    <t>Indicates whther the cost is a one-time/start up cost or a recurring cost. All recurring costs are assumed to be annual unless another (temporal) custom multiplier is specified.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -404,17 +407,95 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Country: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">central or national-level government
+      <t xml:space="preserve">One-time </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">costs are needed once, assumed to be during year 1 or at startup
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Recurring </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>costs are needed multiple times, assumed to be annually unless another (temporal) custom multiplier is specified</t>
+    </r>
+  </si>
+  <si>
+    <t>A custom multiplier that can be used to adjust the cost of the line item, for example, specifying how many times an activity is needed per year, or how many days a meeting is, or how many software licenses are needed.</t>
+  </si>
+  <si>
+    <t>The units associated with the custom multiplier</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>subcategory</t>
+  </si>
+  <si>
+    <t>The category of the cost based on the cost categories defined by GHSS. Please see methods documentation for more detailed definitions</t>
+  </si>
+  <si>
+    <t>The subcategory of the cost based on the cost categories defined by GHSS. Please see methods documentation for more detailed definitions</t>
+  </si>
+  <si>
+    <t>line_item_id</t>
+  </si>
+  <si>
+    <t>A universally unique identifier (UUID) for each line item</t>
+  </si>
+  <si>
+    <t>UUIDs generated using the R id package (https://cran.r-project.org/web/packages/ids/index.html), uuid function</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>The currency, including the year, that the default value is specified in, currently always 2022 USD as noted above</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Country:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> central or national-level government
 </t>
     </r>
     <r>
@@ -492,23 +573,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Population:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Population, used to calculate costs for activities that scale with total population size (e.g., cost per vaccine dose)</t>
-    </r>
-  </si>
-  <si>
-    <t>Indicates whther the cost is a one-time/start up cost or a recurring cost. All recurring costs are assumed to be annual unless another (temporal) custom multiplier is specified.</t>
-  </si>
-  <si>
+      <t xml:space="preserve">Additional HWC/per 1000 population: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The number of additional physicians, nurses, or midwives needed to reach the specified national target (beyond existing workforce); target recommended by WHO is 4.45 doctors, nurses or midwives per 1000 population for operational routine services
+</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -518,17 +595,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">One-time </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">costs are needed once, assumed to be during year 1 or at startup
+      <t xml:space="preserve">PoE: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The number of designated national-level points of entry participating in IHR-related activities
 </t>
     </r>
     <r>
@@ -540,45 +617,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Recurring </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>costs are needed multiple times, assumed to be annually unless another (temporal) custom multiplier is specified</t>
-    </r>
-  </si>
-  <si>
-    <t>A custom multiplier that can be used to adjust the cost of the line item, for example, specifying how many times an activity is needed per year, or how many days a meeting is, or how many software licenses are needed.</t>
-  </si>
-  <si>
-    <t>The units associated with the custom multiplier</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>subcategory</t>
-  </si>
-  <si>
-    <t>The category of the cost based on the cost categories defined by GHSS. Please see methods documentation for more detailed definitions</t>
-  </si>
-  <si>
-    <t>The subcategory of the cost based on the cost categories defined by GHSS. Please see methods documentation for more detailed definitions</t>
-  </si>
-  <si>
-    <t>line_item_id</t>
-  </si>
-  <si>
-    <t>A universally unique identifier (UUID) for each line item</t>
-  </si>
-  <si>
-    <t>UUIDs generated using the R id package (https://cran.r-project.org/web/packages/ids/index.html), uuid function</t>
+      <t xml:space="preserve">Population: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Population, used to calculate costs for activities that scale with total population size (e.g., cost per vaccine dose)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -641,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -657,6 +707,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -972,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1224,10 +1277,10 @@
         <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1235,10 +1288,10 @@
         <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1279,10 +1332,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1290,10 +1343,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1301,21 +1354,21 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1323,10 +1376,10 @@
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1334,10 +1387,10 @@
         <v>39</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1345,10 +1398,10 @@
         <v>39</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1356,10 +1409,10 @@
         <v>39</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1367,10 +1420,10 @@
         <v>39</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1378,10 +1431,10 @@
         <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1389,24 +1442,21 @@
         <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1414,10 +1464,13 @@
         <v>76</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1425,10 +1478,10 @@
         <v>76</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1436,10 +1489,10 @@
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1447,10 +1500,10 @@
         <v>76</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1458,10 +1511,10 @@
         <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1469,10 +1522,10 @@
         <v>76</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1480,10 +1533,10 @@
         <v>76</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1491,10 +1544,10 @@
         <v>76</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1502,38 +1555,35 @@
         <v>76</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="3" t="s">
+    <row r="45" spans="1:4" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>100</v>
+      <c r="D45" s="6" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1541,10 +1591,13 @@
         <v>76</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1552,10 +1605,10 @@
         <v>76</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1563,7 +1616,7 @@
         <v>76</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>101</v>
@@ -1574,10 +1627,10 @@
         <v>76</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1585,10 +1638,10 @@
         <v>76</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1596,10 +1649,10 @@
         <v>76</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1607,9 +1660,20 @@
         <v>76</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add information on WHO member states
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26EFF25-85F0-E94A-A7DD-E70748FE9C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EFB92F-09A6-5B49-91C8-02529B0E5175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="9720" yWindow="2840" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
   <si>
     <t>file</t>
   </si>
@@ -629,6 +629,36 @@
       </rPr>
       <t>Population, used to calculate costs for activities that scale with total population size (e.g., cost per vaccine dose)</t>
     </r>
+  </si>
+  <si>
+    <t>score_numeric</t>
+  </si>
+  <si>
+    <t>score_text</t>
+  </si>
+  <si>
+    <t>If one exists, a written text description corresponding to the numeric score specified</t>
+  </si>
+  <si>
+    <t>who_member_state</t>
+  </si>
+  <si>
+    <t>Whether or not the listed country or geographic area was identified as a WHO member state as of February 2023</t>
+  </si>
+  <si>
+    <t>World Health Organization. Countries overview [Internet]. 2023 [cited 2023 Feb 10]. Available from: https://www.who.int/countries</t>
+  </si>
+  <si>
+    <t>who_region</t>
+  </si>
+  <si>
+    <t>The WHO regional office for the country or geographic area as of February 2023</t>
+  </si>
+  <si>
+    <t>data_team_notes</t>
+  </si>
+  <si>
+    <t>Any additional notes made by the research team during manual extraction, data cleaning, or curation of data</t>
   </si>
 </sst>
 </file>
@@ -691,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -707,9 +737,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,7 +756,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1017,7 +1044,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1025,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1153,7 @@
         <v>59</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>70</v>
@@ -1140,10 +1167,10 @@
         <v>59</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>72</v>
@@ -1151,16 +1178,16 @@
     </row>
     <row r="9" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1168,27 +1195,27 @@
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>6</v>
+      <c r="B11" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1196,13 +1223,13 @@
         <v>23</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1210,13 +1237,13 @@
         <v>23</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1224,13 +1251,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1238,13 +1265,13 @@
         <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1252,57 +1279,63 @@
         <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>102</v>
+        <v>23</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>104</v>
+        <v>74</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>103</v>
+        <v>23</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>105</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1310,10 +1343,13 @@
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1321,10 +1357,10 @@
         <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1332,10 +1368,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1343,10 +1379,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1354,10 +1390,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1365,54 +1401,54 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1420,10 +1456,10 @@
         <v>39</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1431,10 +1467,10 @@
         <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1442,10 +1478,10 @@
         <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1453,57 +1489,54 @@
         <v>39</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1511,10 +1544,13 @@
         <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>71</v>
+        <v>107</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1522,10 +1558,10 @@
         <v>76</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1533,10 +1569,10 @@
         <v>76</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1544,10 +1580,10 @@
         <v>76</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1555,10 +1591,10 @@
         <v>76</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1566,24 +1602,21 @@
         <v>76</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1591,13 +1624,10 @@
         <v>76</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1605,10 +1635,10 @@
         <v>76</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1616,64 +1646,114 @@
         <v>76</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="3" t="s">
+    <row r="53" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B50" s="3" t="s">
+    <row r="54" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B51" s="3" t="s">
+    <row r="55" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B52" s="3" t="s">
+    <row r="56" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B53" s="3" t="s">
+    <row r="57" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add mapping to multiple metric frameworks
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EFB92F-09A6-5B49-91C8-02529B0E5175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34B0ECA-8A5A-C842-965B-F662749EB6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="2840" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="2600" yWindow="1320" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="123">
   <si>
     <t>file</t>
   </si>
@@ -272,9 +272,6 @@
     <t>indicator</t>
   </si>
   <si>
-    <t>score</t>
-  </si>
-  <si>
     <t>attribute</t>
   </si>
   <si>
@@ -372,9 +369,6 @@
   </si>
   <si>
     <t>Any additional references associated with the designation of the line item</t>
-  </si>
-  <si>
-    <t>A unique ID associated with the specified metric, which can be used to join to the metrics.tsv table</t>
   </si>
   <si>
     <t>The requirement specified based on the attribute</t>
@@ -659,6 +653,15 @@
   </si>
   <si>
     <t>Any additional notes made by the research team during manual extraction, data cleaning, or curation of data</t>
+  </si>
+  <si>
+    <t>Where a single line-item corresponding to more than one metric from a given framework (e.g. JEE or SPAR), efforts where made to disambiguate to the extent possible in order to assign each line item to a maximum of one specific metric per framework. For example, a given cost will not be mapped to more than one metric of the JEE. Instead, each line item was mapped to the single most relevant metric per framework.</t>
+  </si>
+  <si>
+    <t>metric_ids</t>
+  </si>
+  <si>
+    <t>A unique ID (or unique IDs) associated with the specified metric(s), which can be used to join to the metrics.tsv table, metrics are listed in a comma serparated list</t>
   </si>
 </sst>
 </file>
@@ -1052,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1083,111 +1086,111 @@
     </row>
     <row r="2" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1251,13 +1254,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1265,13 +1268,13 @@
         <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1307,13 +1310,13 @@
         <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1332,10 +1335,10 @@
         <v>23</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1357,10 +1360,10 @@
         <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1368,10 +1371,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1412,10 +1415,10 @@
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1541,220 +1544,190 @@
     </row>
     <row r="39" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>91</v>
+        <v>122</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="C41" s="4" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="C46" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="4" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="4" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update documentation and ensure data dictionary aligns with actual names in spreadsheet files, add general hospital definition
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34B0ECA-8A5A-C842-965B-F662749EB6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D75CD2E-92E3-0C4B-A374-B49ED898F7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="1320" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="1580" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="fields" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="128">
   <si>
     <t>file</t>
   </si>
@@ -106,15 +106,9 @@
     <t xml:space="preserve">The number of intermediate areas identified by the CIA World Factbook data. Note that while these data can be used to roughly estimate the number of administrative regions per country; this information is best supplemented by local expertise and information on the administrative organization of IHR-related activities. </t>
   </si>
   <si>
-    <t>country.tsv</t>
-  </si>
-  <si>
     <t>unit_costs.tsv</t>
   </si>
   <si>
-    <t>cost</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
   </si>
   <si>
     <t>The unit that the cost is measured in (e.g., per day, per year, per set, etc)</t>
-  </si>
-  <si>
-    <t>assumption</t>
   </si>
   <si>
     <t>Written documentation of any key assumptions associated with the default cost</t>
@@ -212,12 +203,6 @@
     </r>
   </si>
   <si>
-    <t>The name of the default cost</t>
-  </si>
-  <si>
-    <t>A brief written description of the default cost</t>
-  </si>
-  <si>
     <t>detailed_costing.tsv</t>
   </si>
   <si>
@@ -239,9 +224,6 @@
     <t>url</t>
   </si>
   <si>
-    <t>The name of the costed unit, corresponding to a costed unit in unit_costs.tsv</t>
-  </si>
-  <si>
     <t>The subcategory, if any, associated with the items</t>
   </si>
   <si>
@@ -321,9 +303,6 @@
   </si>
   <si>
     <t>Metadata documenting the source (and date) based on which the intermediate area data were determined</t>
-  </si>
-  <si>
-    <t>Currently all intermediate data come from the CIA World Factbook (2022)</t>
   </si>
   <si>
     <t>line_items.tsv</t>
@@ -662,6 +641,42 @@
   </si>
   <si>
     <t>A unique ID (or unique IDs) associated with the specified metric(s), which can be used to join to the metrics.tsv table, metrics are listed in a comma serparated list</t>
+  </si>
+  <si>
+    <t>countries.tsv</t>
+  </si>
+  <si>
+    <t>general_hospital_count</t>
+  </si>
+  <si>
+    <t>Estimated number of general hospitals in the country, if available from OECD (based on most recent data); OECD defines general hospitals as "licensed establishments primarily engaged in providing general diagnostic and medical treatment (both surgical and non-surgical) to inpatients with a wide variety of medical conditions." For more information, including date of last refresh of these data in github, see scripts and documentation in generate-country-data/ directory in github.</t>
+  </si>
+  <si>
+    <t>general_hospital_reference</t>
+  </si>
+  <si>
+    <t>Currently all data are from OECD; For more information, including date of last refresh of these data in github, see scripts and documentation in generate-country-data/ directory in github.</t>
+  </si>
+  <si>
+    <t>Currently all intermediate data come from the CIA World Factbook (2022); For more information, including date of last refresh of these data in github, see scripts and documentation in generate-country-data/ directory in github.</t>
+  </si>
+  <si>
+    <t>The name of the default unit cost</t>
+  </si>
+  <si>
+    <t>A brief written description of the default unit cost</t>
+  </si>
+  <si>
+    <t>assumptions</t>
+  </si>
+  <si>
+    <t>The name of detailed unit cost being calculated from subcomponents, corresponding to a costed unit in unit_costs.tsv</t>
+  </si>
+  <si>
+    <t>cost_per_unit</t>
+  </si>
+  <si>
+    <t>This is somewhat confusing given the name "unit cost" above, but this corresponds specifically to the cost per "item" that is eventually used to calculate a grouped cost</t>
   </si>
 </sst>
 </file>
@@ -712,7 +727,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -720,25 +735,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1055,161 +1134,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="74.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="175.33203125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="74.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="175.33203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="4" t="s">
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="4" t="s">
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="D9" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
@@ -1221,9 +1301,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
@@ -1235,9 +1315,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>7</v>
@@ -1249,37 +1329,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>9</v>
@@ -1291,9 +1371,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>10</v>
@@ -1305,23 +1385,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>8</v>
@@ -1329,407 +1409,467 @@
       <c r="C19" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="B23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="C27" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="C34" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="C35" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="C47" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" s="3" customFormat="1" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+    <row r="49" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="C52" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="C53" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="3" t="s">
+      <c r="C54" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="3" t="s">
+      <c r="C55" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" s="3" t="s">
+      <c r="C56" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
+      <c r="D56" s="9"/>
+    </row>
+    <row r="57" spans="1:4" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
split metric IDs into separate fields for JEE, SPAR, and HEPR to make data easier to work with
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D75CD2E-92E3-0C4B-A374-B49ED898F7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30588F34-1FB7-0046-B6B8-6FF40EDF91DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="760" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="1620" yWindow="7460" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="134">
   <si>
     <t>file</t>
   </si>
@@ -634,15 +634,6 @@
     <t>Any additional notes made by the research team during manual extraction, data cleaning, or curation of data</t>
   </si>
   <si>
-    <t>Where a single line-item corresponding to more than one metric from a given framework (e.g. JEE or SPAR), efforts where made to disambiguate to the extent possible in order to assign each line item to a maximum of one specific metric per framework. For example, a given cost will not be mapped to more than one metric of the JEE. Instead, each line item was mapped to the single most relevant metric per framework.</t>
-  </si>
-  <si>
-    <t>metric_ids</t>
-  </si>
-  <si>
-    <t>A unique ID (or unique IDs) associated with the specified metric(s), which can be used to join to the metrics.tsv table, metrics are listed in a comma serparated list</t>
-  </si>
-  <si>
     <t>countries.tsv</t>
   </si>
   <si>
@@ -677,6 +668,33 @@
   </si>
   <si>
     <t>This is somewhat confusing given the name "unit cost" above, but this corresponds specifically to the cost per "item" that is eventually used to calculate a grouped cost</t>
+  </si>
+  <si>
+    <t>jee3_metric_id</t>
+  </si>
+  <si>
+    <t>A unique ID associated with the specified metric of JEE 3.0</t>
+  </si>
+  <si>
+    <t>spar2_metric_id</t>
+  </si>
+  <si>
+    <t>A unique ID associated with the specified metric of SPAR 2.0</t>
+  </si>
+  <si>
+    <t>hepr_metric_id</t>
+  </si>
+  <si>
+    <t>A unique ID associated with the specified metric of Global Architecture for Health Emergency Preparedness, Response and Resilience (HEPR)</t>
+  </si>
+  <si>
+    <t>Where a single line-item corresponding to more than one metric from a given framework (e.g. JEE or SPAR), efforts where made to disambiguate to the extent possible in order to assign each line item to a maximum of one specific metric per framework. For example, a given cost will not be mapped to more than one metric of the JEE. Instead, each line item was mapped to the single most relevant metric per framework. For more information on the HEPR framework, please see WHO documentation https://www.who.int/emergencies/operations/universal-health---preparedness-review</t>
+  </si>
+  <si>
+    <t>Where a single line-item corresponding to more than one metric from a given framework (e.g. JEE or SPAR), efforts where made to disambiguate to the extent possible in order to assign each line item to a maximum of one specific metric per framework. For example, a given cost will not be mapped to more than one metric of the JEE. Instead, each line item was mapped to the single most relevant metric per framework. For more information on the JEE, please see WHO documentation https://www.who.int/publications/i/item/9789240051980</t>
+  </si>
+  <si>
+    <t>Where a single line-item corresponding to more than one metric from a given framework (e.g. JEE or SPAR), efforts where made to disambiguate to the extent possible in order to assign each line item to a maximum of one specific metric per framework. For example, a given cost will not be mapped to more than one metric of the JEE. Instead, each line item was mapped to the single most relevant metric per framework. For more information on the SPAR, please see WHO documentation https://www.who.int/emergencies/operations/international-health-regulations-monitoring-evaluation-framework/states-parties-self-assessment-annual-reporting</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1275,7 +1293,7 @@
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>4</v>
@@ -1289,7 +1307,7 @@
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
@@ -1303,7 +1321,7 @@
     </row>
     <row r="12" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
@@ -1317,7 +1335,7 @@
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>7</v>
@@ -1331,7 +1349,7 @@
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>106</v>
@@ -1345,7 +1363,7 @@
     </row>
     <row r="15" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>109</v>
@@ -1359,7 +1377,7 @@
     </row>
     <row r="16" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>9</v>
@@ -1373,7 +1391,7 @@
     </row>
     <row r="17" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>10</v>
@@ -1387,7 +1405,7 @@
     </row>
     <row r="18" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>66</v>
@@ -1396,12 +1414,12 @@
         <v>67</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>8</v>
@@ -1413,33 +1431,33 @@
     </row>
     <row r="20" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>111</v>
@@ -1495,7 +1513,7 @@
         <v>38</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D26" s="4"/>
     </row>
@@ -1507,7 +1525,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D27" s="4"/>
     </row>
@@ -1552,7 +1570,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>29</v>
@@ -1579,7 +1597,7 @@
         <v>38</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D33" s="7"/>
     </row>
@@ -1624,13 +1642,13 @@
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1688,13 +1706,13 @@
         <v>68</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1702,34 +1720,38 @@
         <v>68</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D43" s="4"/>
+        <v>128</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="44" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="4"/>
+        <v>130</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="45" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D45" s="4"/>
     </row>
@@ -1738,10 +1760,10 @@
         <v>68</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D46" s="4"/>
     </row>
@@ -1750,71 +1772,71 @@
         <v>68</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:4" s="3" customFormat="1" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>102</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" ht="155" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D50" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="51" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D51" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="52" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>91</v>
@@ -1826,7 +1848,7 @@
         <v>68</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>92</v>
@@ -1838,10 +1860,10 @@
         <v>68</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D54" s="4"/>
     </row>
@@ -1850,26 +1872,50 @@
         <v>68</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B58" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C58" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="57" spans="1:4" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:4" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update costing of healthcare workers, calculate by per capita
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30588F34-1FB7-0046-B6B8-6FF40EDF91DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C600EBC-B451-1640-89C5-A84CEC690D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="7460" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="1620" yWindow="1500" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -1154,7 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add info on 2022 spar scores, clean up documentation and data dictionary
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C600EBC-B451-1640-89C5-A84CEC690D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B73D9DA-13DC-624D-B99D-55FEC93E0FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1500" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
+    <workbookView xWindow="2820" yWindow="4380" windowWidth="27640" windowHeight="16620" xr2:uid="{594009AC-F5D3-6641-BBD5-6F8456B11744}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="154">
   <si>
     <t>file</t>
   </si>
@@ -695,6 +695,66 @@
   </si>
   <si>
     <t>Where a single line-item corresponding to more than one metric from a given framework (e.g. JEE or SPAR), efforts where made to disambiguate to the extent possible in order to assign each line item to a maximum of one specific metric per framework. For example, a given cost will not be mapped to more than one metric of the JEE. Instead, each line item was mapped to the single most relevant metric per framework. For more information on the SPAR, please see WHO documentation https://www.who.int/emergencies/operations/international-health-regulations-monitoring-evaluation-framework/states-parties-self-assessment-annual-reporting</t>
+  </si>
+  <si>
+    <t>spar2022_total_average</t>
+  </si>
+  <si>
+    <t>The average of all SPAR scores reported in 2022, as reported and calculated by WHO</t>
+  </si>
+  <si>
+    <t>World Health Organization. e-SPAR Public [Internet]. [cited 2023 May 5]. Available from: https://extranet.who.int/e-spar/</t>
+  </si>
+  <si>
+    <t>spar_2022_human_resources_ihr</t>
+  </si>
+  <si>
+    <t>The score that the country reported for the indicator C.6.1 (Human resources for implementation of IHR) in the year 2022, as reported by WHO</t>
+  </si>
+  <si>
+    <t>doctor_consultations_per_capita</t>
+  </si>
+  <si>
+    <t>doctors_consultation_reference</t>
+  </si>
+  <si>
+    <t>mds_per_10000capita</t>
+  </si>
+  <si>
+    <t>mds_per_10000capita_reference</t>
+  </si>
+  <si>
+    <t>nurses_midwives_per_10000capita</t>
+  </si>
+  <si>
+    <t>nurses_midwives_per_10000capita_reference</t>
+  </si>
+  <si>
+    <t>Doctors' consultations (indicator) [Internet]. doi: 10.1787/173dcf26-en. [cited 2023 April 14] (Accessed on 14 April 2023). Available from: https://data.oecd.org/healthcare/doctors-consultations.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The estimated number of doctor's consultations based on data reported from OECD. From OECD: "This indicator presents data on the number of consultations patients have with doctors in a given year. Consultations with doctors can take place in doctors’ offices or clinics, in hospital outpatient departments or, in some cases, in patients’ own homes. Consultations with doctors refer to the number of contacts with physicians, both generalists and specialists. There are variations across countries in the coverage of different types of consultations, notably in outpatient departments of hospitals. The data come from administrative sources or surveys, depending on the country. This indicator is measured per capita." </t>
+  </si>
+  <si>
+    <t>World Health Organization. Global Health Workforce statistics database [Internet]. [cited 2023 Jan 13]. Available from: https://www.who.int/data/gho/data/themes/topics/health-workforce</t>
+  </si>
+  <si>
+    <t>Currently all data are from WHO; For more information, including date of last refresh of these data in github, see scripts and documentation in generate-country-data/ directory in github.</t>
+  </si>
+  <si>
+    <t>The number of MDs per 10,000 population as reported by the WHO Global Health Workforce statistics database</t>
+  </si>
+  <si>
+    <t>The number of nurses and widwives per 10,000 population as reported by the WHO Global Health Workforce statistics database</t>
+  </si>
+  <si>
+    <t>Metadata documenting the source (and date) based on which the field "nurses_midwives_per_10000capita" was calculated</t>
+  </si>
+  <si>
+    <t>Metadata documenting the source (and date) based on which the field "mds_per_10000capita" was calculated</t>
+  </si>
+  <si>
+    <t>Metadata documenting the source (and date) based on which the field "doctor_consultations_per_capita" was calculated</t>
   </si>
 </sst>
 </file>
@@ -745,7 +805,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -796,11 +856,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -837,6 +910,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,16 +1231,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2F949D-1C6E-D64D-BDD2-DA2A42BB178B}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="74.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="175.33203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="1"/>
@@ -1380,13 +1459,13 @@
         <v>113</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1394,13 +1473,13 @@
         <v>113</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>10</v>
+        <v>137</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>22</v>
+        <v>138</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1408,13 +1487,13 @@
         <v>113</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>118</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1422,399 +1501,409 @@
         <v>113</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="24" spans="1:4" s="3" customFormat="1" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="4"/>
+      <c r="B24" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="25" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="3" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B31" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>124</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>39</v>
+        <v>121</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>99</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>125</v>
+        <v>35</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>132</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>133</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>129</v>
+        <v>37</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>131</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D45" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="46" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1822,13 +1911,13 @@
         <v>68</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1836,22 +1925,24 @@
         <v>68</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D52" s="4"/>
+        <v>130</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="53" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D53" s="4"/>
     </row>
@@ -1860,10 +1951,10 @@
         <v>68</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D54" s="4"/>
     </row>
@@ -1872,10 +1963,10 @@
         <v>68</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D55" s="4"/>
     </row>
@@ -1884,10 +1975,10 @@
         <v>68</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D56" s="4"/>
     </row>
@@ -1896,26 +1987,126 @@
         <v>68</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4" s="3" customFormat="1" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64" s="4"/>
+    </row>
+    <row r="65" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+      <c r="D65" s="4"/>
+    </row>
+    <row r="66" spans="1:4" s="3" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B66" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D58" s="9"/>
-    </row>
-    <row r="59" spans="1:4" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="D66" s="9"/>
+    </row>
+    <row r="67" spans="1:4" ht="90" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>